<commit_message>
handling of dates as string done. tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/diff_milestone_data_formats_master_2_2020.xlsx
+++ b/tests/resources/diff_milestone_data_formats_master_2_2020.xlsx
@@ -34,37 +34,37 @@
     <t xml:space="preserve">Apollo 13</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6</t>
+    <t xml:space="preserve">Assurance MM1</t>
   </si>
   <si>
     <t xml:space="preserve">Gateway Review 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 LoD</t>
+    <t xml:space="preserve">Assurance MM1 LoD</t>
   </si>
   <si>
     <t xml:space="preserve">(2) IPA Gate 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 Version No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assurance MM6 Original Baseline</t>
+    <t xml:space="preserve">Assurance MM1 Version No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assurance MM1 Original Baseline</t>
   </si>
   <si>
     <t xml:space="preserve">26/04/2027</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 Forecast - Actual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assurance MM6 Status</t>
+    <t xml:space="preserve">Assurance MM1 Forecast - Actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assurance MM1 Status</t>
   </si>
   <si>
     <t xml:space="preserve">Live</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 Notes</t>
+    <t xml:space="preserve">Assurance MM1 Notes</t>
   </si>
   <si>
     <t xml:space="preserve">indicative dates tbc</t>
@@ -228,10 +228,10 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="36.17"/>
   </cols>

</xml_diff>

<commit_message>
further refactoring of milestonedata class
</commit_message>
<xml_diff>
--- a/tests/resources/diff_milestone_data_formats_master_2_2020.xlsx
+++ b/tests/resources/diff_milestone_data_formats_master_2_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -146,9 +146,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -215,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,6 +230,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,10 +257,10 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="36.17"/>
   </cols>
@@ -338,8 +343,8 @@
       <c r="C6" s="3" t="n">
         <v>47178</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
+      <c r="D6" s="4" t="n">
+        <v>46480</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>